<commit_message>
adding iteration 2 charts
</commit_message>
<xml_diff>
--- a/charts/BurndownCharts.xlsx
+++ b/charts/BurndownCharts.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="IterationBurndown" sheetId="1" r:id="rId1"/>
     <sheet name="DailyBurndown_Iteration_1" sheetId="2" r:id="rId2"/>
+    <sheet name="DailyBurndown_Iteration_2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>Iteration</t>
   </si>
@@ -49,10 +50,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,14 +92,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -207,29 +228,35 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>IterationBurndown!$A$2:$A$23</c:f>
+              <c:f>IterationBurndown!$A$2:$A$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>IterationBurndown!$C$2:$C$23</c:f>
+              <c:f>IterationBurndown!$C$2:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>36.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>36.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -273,30 +300,36 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>IterationBurndown!$A$2:$A$23</c:f>
+              <c:f>IterationBurndown!$A$2:$A$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>IterationBurndown!$B$2:$B$23</c:f>
+              <c:f>IterationBurndown!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>36.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -311,14 +344,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-759491696"/>
-        <c:axId val="-759818816"/>
+        <c:axId val="1716335408"/>
+        <c:axId val="1817313520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-759491696"/>
+        <c:axId val="1716335408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.0"/>
+          <c:max val="2.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -392,6 +425,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -428,14 +462,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-759818816"/>
+        <c:crossAx val="1817313520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1.0"/>
         <c:minorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-759818816"/>
+        <c:axId val="1817313520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -547,7 +581,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-759491696"/>
+        <c:crossAx val="1716335408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1.0"/>
@@ -931,11 +965,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-758458688"/>
-        <c:axId val="-758456640"/>
+        <c:axId val="1718565312"/>
+        <c:axId val="1718568704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-758458688"/>
+        <c:axId val="1718565312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1034,7 +1068,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-758456640"/>
+        <c:crossAx val="1718568704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1042,7 +1076,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-758456640"/>
+        <c:axId val="1718568704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1148,7 +1182,608 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-758458688"/>
+        <c:crossAx val="1718565312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="1.0"/>
+        <c:minorUnit val="0.5"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Daily Burndown</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> - Iteration 2 </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DailyBurndown_Iteration_2!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Points</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>DailyBurndown_Iteration_1!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>43178.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43179.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43180.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43181.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43182.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43192.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43193.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43194.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43195.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43196.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>DailyBurndown_Iteration_2!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DailyBurndown_Iteration_2!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remaining Points in Iteration</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>DailyBurndown_Iteration_1!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>43178.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43179.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43180.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43181.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43182.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43192.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43193.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43194.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43195.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43196.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>DailyBurndown_Iteration_2!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1862359488"/>
+        <c:axId val="1851694240"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1862359488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Date</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1851694240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1851694240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Points Remaining</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1862359488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
@@ -1311,6 +1946,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1828,6 +2503,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2397,6 +3588,43 @@
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>387350</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2676,10 +3904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2717,6 +3945,17 @@
         <v>34</v>
       </c>
       <c r="C3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>31</v>
+      </c>
+      <c r="C4">
         <v>36</v>
       </c>
     </row>
@@ -2731,8 +3970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2865,4 +4104,141 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>43199</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>43200</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>43201</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>43202</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>43203</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>43206</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>43207</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>43208</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>43209</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>43210</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updating charts for final iteration
</commit_message>
<xml_diff>
--- a/charts/BurndownCharts.xlsx
+++ b/charts/BurndownCharts.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="IterationBurndown" sheetId="1" r:id="rId1"/>
     <sheet name="DailyBurndown_Iteration_1" sheetId="2" r:id="rId2"/>
     <sheet name="DailyBurndown_Iteration_2" sheetId="3" r:id="rId3"/>
+    <sheet name="DailyBurndown_Iteration_3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
   <si>
     <t>Iteration</t>
   </si>
@@ -228,10 +229,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>IterationBurndown!$A$2:$A$4</c:f>
+              <c:f>IterationBurndown!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -240,24 +241,30 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>IterationBurndown!$C$2:$C$4</c:f>
+              <c:f>IterationBurndown!$C$2:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>36.0</c:v>
+                  <c:v>38.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36.0</c:v>
+                  <c:v>37.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.0</c:v>
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -300,10 +307,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>IterationBurndown!$A$2:$A$4</c:f>
+              <c:f>IterationBurndown!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -312,24 +319,30 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>IterationBurndown!$B$2:$B$4</c:f>
+              <c:f>IterationBurndown!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>36.0</c:v>
+                  <c:v>37.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>34.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -344,14 +357,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1716335408"/>
-        <c:axId val="1817313520"/>
+        <c:axId val="1055441888"/>
+        <c:axId val="1099380656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1716335408"/>
+        <c:axId val="1055441888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="2.0"/>
+          <c:max val="3.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -462,16 +475,17 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1817313520"/>
+        <c:crossAx val="1099380656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1.0"/>
         <c:minorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1817313520"/>
+        <c:axId val="1099380656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="18.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -581,7 +595,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1716335408"/>
+        <c:crossAx val="1055441888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1.0"/>
@@ -965,11 +979,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1718565312"/>
-        <c:axId val="1718568704"/>
+        <c:axId val="1171357488"/>
+        <c:axId val="1171361248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1718565312"/>
+        <c:axId val="1171357488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1068,7 +1082,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1718568704"/>
+        <c:crossAx val="1171361248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1076,7 +1090,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1718568704"/>
+        <c:axId val="1171361248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1182,7 +1196,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1718565312"/>
+        <c:crossAx val="1171357488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
@@ -1373,39 +1387,39 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>DailyBurndown_Iteration_1!$A$2:$A$11</c:f>
+              <c:f>DailyBurndown_Iteration_2!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>43178.0</c:v>
+                  <c:v>43199.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43179.0</c:v>
+                  <c:v>43200.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43180.0</c:v>
+                  <c:v>43201.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43181.0</c:v>
+                  <c:v>43202.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43182.0</c:v>
+                  <c:v>43203.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43192.0</c:v>
+                  <c:v>43206.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43193.0</c:v>
+                  <c:v>43207.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43194.0</c:v>
+                  <c:v>43208.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43195.0</c:v>
+                  <c:v>43209.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43196.0</c:v>
+                  <c:v>43210.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1479,39 +1493,39 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>DailyBurndown_Iteration_1!$A$2:$A$11</c:f>
+              <c:f>DailyBurndown_Iteration_2!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>43178.0</c:v>
+                  <c:v>43199.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43179.0</c:v>
+                  <c:v>43200.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43180.0</c:v>
+                  <c:v>43201.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43181.0</c:v>
+                  <c:v>43202.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43182.0</c:v>
+                  <c:v>43203.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43192.0</c:v>
+                  <c:v>43206.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43193.0</c:v>
+                  <c:v>43207.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43194.0</c:v>
+                  <c:v>43208.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43195.0</c:v>
+                  <c:v>43209.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43196.0</c:v>
+                  <c:v>43210.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1566,11 +1580,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1862359488"/>
-        <c:axId val="1851694240"/>
+        <c:axId val="1172368784"/>
+        <c:axId val="1172372816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1862359488"/>
+        <c:axId val="1172368784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1669,7 +1683,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1851694240"/>
+        <c:crossAx val="1172372816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1677,7 +1691,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1851694240"/>
+        <c:axId val="1172372816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1783,7 +1797,608 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1862359488"/>
+        <c:crossAx val="1172368784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="1.0"/>
+        <c:minorUnit val="0.5"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Daily Burndown</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> - Iteration 3 </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DailyBurndown_Iteration_3!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Points</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>DailyBurndown_Iteration_3!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>43213.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43214.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43215.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43216.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43217.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43218.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43219.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43220.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43221.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43222.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>DailyBurndown_Iteration_3!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DailyBurndown_Iteration_3!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remaining Points in Iteration</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>DailyBurndown_Iteration_3!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>43213.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43214.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43215.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43216.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43217.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43218.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43219.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43220.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43221.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43222.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>DailyBurndown_Iteration_3!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1171969264"/>
+        <c:axId val="1171972656"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1171969264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Date</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1171972656"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1171972656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Points Remaining</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1171969264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
@@ -1986,6 +2601,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3019,6 +3674,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3605,6 +4776,43 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>387350</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3904,10 +5112,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3931,10 +5139,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C2">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -3945,7 +5153,7 @@
         <v>34</v>
       </c>
       <c r="C3">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -3956,7 +5164,18 @@
         <v>31</v>
       </c>
       <c r="C4">
-        <v>36</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -4110,8 +5329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4241,4 +5460,141 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>43213</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>43214</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>43215</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>43216</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>43217</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>43218</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>43219</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>43220</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>43221</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>43222</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>